<commit_message>
Added Excel with all API calls + modified YML
</commit_message>
<xml_diff>
--- a/src/test/resources/rest/Regres.xlsx
+++ b/src/test/resources/rest/Regres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajinkya\Downloads\microservices-lowcode-testautomation-master\microservices-lowcode-testautomation-master\rest-get\src\test\resources\rest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AjinkyaKunjir\Konverter\src\test\resources\rest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B53A8A-C866-432A-B87E-C2CFD3584549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150C41C0-66BB-4870-BB87-1D8FBFBB0AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="REST-API-Get" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -95,6 +95,66 @@
   </si>
   <si>
     <t>ep</t>
+  </si>
+  <si>
+    <t>Test one-POST</t>
+  </si>
+  <si>
+    <t>Post users</t>
+  </si>
+  <si>
+    <t>https://reqres.in/api/users</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>name=venom</t>
+  </si>
+  <si>
+    <t>RequestContent</t>
+  </si>
+  <si>
+    <t>{
+    "name": "venom",
+    "job": "snake"
+}</t>
+  </si>
+  <si>
+    <t>Test one- PUT</t>
+  </si>
+  <si>
+    <t>Put user</t>
+  </si>
+  <si>
+    <t>https://reqres.in/api/users/2</t>
+  </si>
+  <si>
+    <t>PUT</t>
+  </si>
+  <si>
+    <t>{
+    "name": "venom",
+    "job": "zion resident"
+}</t>
+  </si>
+  <si>
+    <t>Test one - PATCH</t>
+  </si>
+  <si>
+    <t>PATCH user</t>
+  </si>
+  <si>
+    <t>PATCH</t>
+  </si>
+  <si>
+    <t>Test one - DELETE</t>
+  </si>
+  <si>
+    <t>DELETE user</t>
+  </si>
+  <si>
+    <t>DELETE</t>
   </si>
 </sst>
 </file>
@@ -191,7 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -206,6 +266,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -522,27 +585,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="65.453125" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" customWidth="1"/>
+    <col min="10" max="10" width="24.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" customWidth="1"/>
+    <col min="12" max="12" width="65.44140625" customWidth="1"/>
+    <col min="13" max="13" width="24.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,16 +636,19 @@
         <v>10</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -609,8 +677,143 @@
         <v>19</v>
       </c>
       <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>201</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>204</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>